<commit_message>
Insert/Delete column in a table
</commit_message>
<xml_diff>
--- a/resources/student.xlsx
+++ b/resources/student.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fasulu\Documents\UiPath\InsertDeleteFilterInTableActivity\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C265939-02FA-4FF1-9341-75834413A875}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62673F40-D6B6-464F-8B78-D4C53969B00E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="30">
   <si>
     <t>Name</t>
   </si>
@@ -125,9 +125,6 @@
   </si>
   <si>
     <t>Roll No.</t>
-  </si>
-  <si>
-    <t>Grade</t>
   </si>
 </sst>
 </file>
@@ -209,38 +206,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="12">
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <border>
-        <bottom style="double">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
+  <dxfs count="11">
     <dxf>
       <font>
         <b val="0"/>
@@ -456,6 +422,13 @@
       </fill>
     </dxf>
     <dxf>
+      <border>
+        <bottom style="double">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
       <font>
         <b/>
         <i val="0"/>
@@ -494,18 +467,17 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00C34460-F8BC-43E3-846B-020ADE41E02E}" name="Marks" displayName="Marks" ref="A1:H15" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10" headerRowBorderDxfId="1" tableBorderDxfId="9">
-  <autoFilter ref="A1:H15" xr:uid="{00C34460-F8BC-43E3-846B-020ADE41E02E}"/>
-  <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{09D84CF5-DC88-4319-8469-03FC95A44745}" name="Roll No." dataDxfId="8"/>
-    <tableColumn id="2" xr3:uid="{CF90F1A0-AE5B-4712-92AF-480AE42AC045}" name="Name" dataDxfId="7"/>
-    <tableColumn id="3" xr3:uid="{E43BA2A3-21F0-48D9-A7C7-2014A80DBD3B}" name="Dept" dataDxfId="6"/>
-    <tableColumn id="8" xr3:uid="{7397DFF0-8B07-45FB-B7DB-1D7C0272BE1C}" name="Grade" dataDxfId="0"/>
-    <tableColumn id="4" xr3:uid="{7609AFC0-ECE2-4B7A-95D7-B5BD904C6450}" name="Sem 1" dataDxfId="5"/>
-    <tableColumn id="5" xr3:uid="{F45E1EA6-ECF6-4D80-A986-2429DD61057F}" name="Sem 2" dataDxfId="4"/>
-    <tableColumn id="6" xr3:uid="{40EA00DE-CB12-443D-B8BA-273510C6DE7F}" name="Sem 3" dataDxfId="3"/>
-    <tableColumn id="7" xr3:uid="{8A20179E-9E2B-42C1-9BB9-697F6BDE0B2F}" name="Avg" dataDxfId="2">
-      <calculatedColumnFormula>SUM(E2:G2)/3</calculatedColumnFormula>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00C34460-F8BC-43E3-846B-020ADE41E02E}" name="Marks" displayName="Marks" ref="A1:G15" totalsRowShown="0" headerRowDxfId="10" dataDxfId="8" headerRowBorderDxfId="9" tableBorderDxfId="7">
+  <autoFilter ref="A1:G15" xr:uid="{00C34460-F8BC-43E3-846B-020ADE41E02E}"/>
+  <tableColumns count="7">
+    <tableColumn id="1" xr3:uid="{09D84CF5-DC88-4319-8469-03FC95A44745}" name="Roll No." dataDxfId="6"/>
+    <tableColumn id="2" xr3:uid="{CF90F1A0-AE5B-4712-92AF-480AE42AC045}" name="Name" dataDxfId="5"/>
+    <tableColumn id="3" xr3:uid="{E43BA2A3-21F0-48D9-A7C7-2014A80DBD3B}" name="Dept" dataDxfId="4"/>
+    <tableColumn id="4" xr3:uid="{7609AFC0-ECE2-4B7A-95D7-B5BD904C6450}" name="Sem 1" dataDxfId="3"/>
+    <tableColumn id="5" xr3:uid="{F45E1EA6-ECF6-4D80-A986-2429DD61057F}" name="Sem 2" dataDxfId="2"/>
+    <tableColumn id="6" xr3:uid="{40EA00DE-CB12-443D-B8BA-273510C6DE7F}" name="Sem 3" dataDxfId="1"/>
+    <tableColumn id="7" xr3:uid="{8A20179E-9E2B-42C1-9BB9-697F6BDE0B2F}" name="Avg" dataDxfId="0">
+      <calculatedColumnFormula>SUM(D2:F2)/3</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -775,7 +747,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q15"/>
+  <dimension ref="A1:P15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="G17" sqref="G17"/>
@@ -793,7 +765,7 @@
     <col min="12" max="12" width="14.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="6" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" s="6" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
         <v>29</v>
       </c>
@@ -804,43 +776,40 @@
         <v>1</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>30</v>
+        <v>3</v>
       </c>
       <c r="E1" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="K1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="L1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="M1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="N1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="O1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="7" t="s">
+      <c r="P1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="K1" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="L1" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="M1" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="N1" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="O1" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="P1" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q1" s="5" t="s">
-        <v>5</v>
-      </c>
     </row>
-    <row r="2" spans="1:17" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1011</v>
       </c>
@@ -850,7 +819,9 @@
       <c r="C2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="3"/>
+      <c r="D2" s="4">
+        <v>18</v>
+      </c>
       <c r="E2" s="4">
         <v>18</v>
       </c>
@@ -858,21 +829,21 @@
         <v>18</v>
       </c>
       <c r="G2" s="4">
-        <v>18</v>
-      </c>
-      <c r="H2" s="4">
-        <f t="shared" ref="H2:H15" si="0">SUM(E2:G2)/3</f>
-        <v>18</v>
-      </c>
-      <c r="K2" s="2">
+        <f t="shared" ref="G2:G15" si="0">SUM(D2:F2)/3</f>
+        <v>18</v>
+      </c>
+      <c r="J2" s="2">
         <v>1011</v>
       </c>
+      <c r="K2" s="3" t="s">
+        <v>8</v>
+      </c>
       <c r="L2" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="M2" s="3" t="s">
         <v>9</v>
       </c>
+      <c r="M2" s="4">
+        <v>18</v>
+      </c>
       <c r="N2" s="4">
         <v>18</v>
       </c>
@@ -880,14 +851,11 @@
         <v>18</v>
       </c>
       <c r="P2" s="4">
-        <v>18</v>
-      </c>
-      <c r="Q2" s="4">
-        <f t="shared" ref="Q2:Q15" si="1">SUM(N2:P2)/3</f>
+        <f t="shared" ref="P2:P15" si="1">SUM(M2:O2)/3</f>
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>1018</v>
       </c>
@@ -897,44 +865,43 @@
       <c r="C3" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="3"/>
+      <c r="D3" s="4">
+        <v>10</v>
+      </c>
       <c r="E3" s="4">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="F3" s="4">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="G3" s="4">
-        <v>19</v>
-      </c>
-      <c r="H3" s="4">
         <f t="shared" si="0"/>
         <v>14.666666666666666</v>
       </c>
-      <c r="K3" s="2">
+      <c r="J3" s="2">
         <v>1018</v>
       </c>
+      <c r="K3" s="3" t="s">
+        <v>10</v>
+      </c>
       <c r="L3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="M3" s="4">
         <v>10</v>
       </c>
-      <c r="M3" s="3" t="s">
-        <v>11</v>
-      </c>
       <c r="N3" s="4">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="O3" s="4">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="P3" s="4">
-        <v>19</v>
-      </c>
-      <c r="Q3" s="4">
         <f t="shared" si="1"/>
         <v>14.666666666666666</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>1015</v>
       </c>
@@ -944,44 +911,43 @@
       <c r="C4" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="D4" s="3"/>
+      <c r="D4" s="4">
+        <v>18</v>
+      </c>
       <c r="E4" s="4">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="F4" s="4">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="G4" s="4">
-        <v>18</v>
-      </c>
-      <c r="H4" s="4">
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
-      <c r="K4" s="2">
+      <c r="J4" s="2">
         <v>1015</v>
       </c>
+      <c r="K4" s="3" t="s">
+        <v>19</v>
+      </c>
       <c r="L4" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="M4" s="3" t="s">
         <v>20</v>
       </c>
+      <c r="M4" s="4">
+        <v>18</v>
+      </c>
       <c r="N4" s="4">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="O4" s="4">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="P4" s="4">
-        <v>18</v>
-      </c>
-      <c r="Q4" s="4">
         <f t="shared" si="1"/>
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>1020</v>
       </c>
@@ -991,44 +957,43 @@
       <c r="C5" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="3"/>
+      <c r="D5" s="4">
+        <v>2</v>
+      </c>
       <c r="E5" s="4">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="F5" s="4">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G5" s="4">
-        <v>4</v>
-      </c>
-      <c r="H5" s="4">
         <f t="shared" si="0"/>
         <v>3.6666666666666665</v>
       </c>
-      <c r="K5" s="2">
+      <c r="J5" s="2">
         <v>1020</v>
       </c>
+      <c r="K5" s="3" t="s">
+        <v>23</v>
+      </c>
       <c r="L5" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="M5" s="3" t="s">
         <v>11</v>
       </c>
+      <c r="M5" s="4">
+        <v>2</v>
+      </c>
       <c r="N5" s="4">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="O5" s="4">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="P5" s="4">
-        <v>4</v>
-      </c>
-      <c r="Q5" s="4">
         <f t="shared" si="1"/>
         <v>3.6666666666666665</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>1022</v>
       </c>
@@ -1038,44 +1003,43 @@
       <c r="C6" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="D6" s="3"/>
+      <c r="D6" s="4">
+        <v>12</v>
+      </c>
       <c r="E6" s="4">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="F6" s="4">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="G6" s="4">
-        <v>20</v>
-      </c>
-      <c r="H6" s="4">
         <f t="shared" si="0"/>
         <v>16.666666666666668</v>
       </c>
-      <c r="K6" s="2">
+      <c r="J6" s="2">
         <v>1022</v>
       </c>
+      <c r="K6" s="3" t="s">
+        <v>25</v>
+      </c>
       <c r="L6" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="M6" s="3" t="s">
         <v>27</v>
       </c>
+      <c r="M6" s="4">
+        <v>12</v>
+      </c>
       <c r="N6" s="4">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="O6" s="4">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="P6" s="4">
-        <v>20</v>
-      </c>
-      <c r="Q6" s="4">
         <f t="shared" si="1"/>
         <v>16.666666666666668</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>1021</v>
       </c>
@@ -1085,44 +1049,43 @@
       <c r="C7" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="D7" s="3"/>
+      <c r="D7" s="4">
+        <v>15</v>
+      </c>
       <c r="E7" s="4">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="F7" s="4">
+        <v>20</v>
+      </c>
+      <c r="G7" s="4">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="J7" s="2">
+        <v>1021</v>
+      </c>
+      <c r="K7" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="L7" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="M7" s="4">
+        <v>15</v>
+      </c>
+      <c r="N7" s="4">
         <v>19</v>
       </c>
-      <c r="G7" s="4">
+      <c r="O7" s="4">
         <v>20</v>
       </c>
-      <c r="H7" s="4">
-        <f t="shared" si="0"/>
-        <v>18</v>
-      </c>
-      <c r="K7" s="2">
-        <v>1021</v>
-      </c>
-      <c r="L7" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="M7" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="N7" s="4">
-        <v>15</v>
-      </c>
-      <c r="O7" s="4">
-        <v>19</v>
-      </c>
       <c r="P7" s="4">
-        <v>20</v>
-      </c>
-      <c r="Q7" s="4">
         <f t="shared" si="1"/>
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>1010</v>
       </c>
@@ -1132,44 +1095,43 @@
       <c r="C8" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D8" s="3"/>
+      <c r="D8" s="4">
+        <v>19</v>
+      </c>
       <c r="E8" s="4">
         <v>19</v>
       </c>
       <c r="F8" s="4">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G8" s="4">
-        <v>20</v>
-      </c>
-      <c r="H8" s="4">
         <f t="shared" si="0"/>
         <v>19.333333333333332</v>
       </c>
-      <c r="K8" s="2">
+      <c r="J8" s="2">
         <v>1010</v>
       </c>
+      <c r="K8" s="3" t="s">
+        <v>17</v>
+      </c>
       <c r="L8" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="M8" s="3" t="s">
         <v>16</v>
+      </c>
+      <c r="M8" s="4">
+        <v>19</v>
       </c>
       <c r="N8" s="4">
         <v>19</v>
       </c>
       <c r="O8" s="4">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="P8" s="4">
-        <v>20</v>
-      </c>
-      <c r="Q8" s="4">
         <f t="shared" si="1"/>
         <v>19.333333333333332</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>1019</v>
       </c>
@@ -1179,44 +1141,43 @@
       <c r="C9" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D9" s="3"/>
+      <c r="D9" s="4">
+        <v>12</v>
+      </c>
       <c r="E9" s="4">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F9" s="4">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="G9" s="4">
-        <v>15</v>
-      </c>
-      <c r="H9" s="4">
         <f t="shared" si="0"/>
         <v>13.333333333333334</v>
       </c>
-      <c r="K9" s="2">
+      <c r="J9" s="2">
         <v>1019</v>
       </c>
+      <c r="K9" s="3" t="s">
+        <v>12</v>
+      </c>
       <c r="L9" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="M9" s="4">
         <v>12</v>
       </c>
-      <c r="M9" s="3" t="s">
-        <v>11</v>
-      </c>
       <c r="N9" s="4">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="O9" s="4">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="P9" s="4">
-        <v>15</v>
-      </c>
-      <c r="Q9" s="4">
         <f t="shared" si="1"/>
         <v>13.333333333333334</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>1016</v>
       </c>
@@ -1226,44 +1187,43 @@
       <c r="C10" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D10" s="3"/>
+      <c r="D10" s="4">
+        <v>17</v>
+      </c>
       <c r="E10" s="4">
+        <v>18</v>
+      </c>
+      <c r="F10" s="4">
+        <v>19</v>
+      </c>
+      <c r="G10" s="4">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="J10" s="2">
+        <v>1016</v>
+      </c>
+      <c r="K10" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="L10" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="M10" s="4">
         <v>17</v>
       </c>
-      <c r="F10" s="4">
-        <v>18</v>
-      </c>
-      <c r="G10" s="4">
+      <c r="N10" s="4">
+        <v>18</v>
+      </c>
+      <c r="O10" s="4">
         <v>19</v>
       </c>
-      <c r="H10" s="4">
-        <f t="shared" si="0"/>
-        <v>18</v>
-      </c>
-      <c r="K10" s="2">
-        <v>1016</v>
-      </c>
-      <c r="L10" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="M10" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="N10" s="4">
-        <v>17</v>
-      </c>
-      <c r="O10" s="4">
-        <v>18</v>
-      </c>
       <c r="P10" s="4">
-        <v>19</v>
-      </c>
-      <c r="Q10" s="4">
         <f t="shared" si="1"/>
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>1012</v>
       </c>
@@ -1273,44 +1233,43 @@
       <c r="C11" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D11" s="3"/>
+      <c r="D11" s="4">
+        <v>15</v>
+      </c>
       <c r="E11" s="4">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="F11" s="4">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="G11" s="4">
-        <v>18</v>
-      </c>
-      <c r="H11" s="4">
         <f t="shared" si="0"/>
         <v>16.666666666666668</v>
       </c>
-      <c r="K11" s="2">
+      <c r="J11" s="2">
         <v>1012</v>
       </c>
+      <c r="K11" s="3" t="s">
+        <v>13</v>
+      </c>
       <c r="L11" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="M11" s="3" t="s">
         <v>14</v>
       </c>
+      <c r="M11" s="4">
+        <v>15</v>
+      </c>
       <c r="N11" s="4">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="O11" s="4">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="P11" s="4">
-        <v>18</v>
-      </c>
-      <c r="Q11" s="4">
         <f t="shared" si="1"/>
         <v>16.666666666666668</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>1013</v>
       </c>
@@ -1320,44 +1279,43 @@
       <c r="C12" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D12" s="3"/>
+      <c r="D12" s="4">
+        <v>14</v>
+      </c>
       <c r="E12" s="4">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F12" s="4">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="G12" s="4">
-        <v>19</v>
-      </c>
-      <c r="H12" s="4">
         <f t="shared" si="0"/>
         <v>15.333333333333334</v>
       </c>
-      <c r="K12" s="2">
+      <c r="J12" s="2">
         <v>1013</v>
       </c>
+      <c r="K12" s="3" t="s">
+        <v>15</v>
+      </c>
       <c r="L12" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="M12" s="3" t="s">
         <v>7</v>
       </c>
+      <c r="M12" s="4">
+        <v>14</v>
+      </c>
       <c r="N12" s="4">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="O12" s="4">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="P12" s="4">
-        <v>19</v>
-      </c>
-      <c r="Q12" s="4">
         <f t="shared" si="1"/>
         <v>15.333333333333334</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>1014</v>
       </c>
@@ -1367,44 +1325,43 @@
       <c r="C13" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D13" s="3"/>
+      <c r="D13" s="4">
+        <v>17</v>
+      </c>
       <c r="E13" s="4">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="F13" s="4">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="G13" s="4">
-        <v>18</v>
-      </c>
-      <c r="H13" s="4">
         <f t="shared" si="0"/>
         <v>16.666666666666668</v>
       </c>
-      <c r="K13" s="2">
+      <c r="J13" s="2">
         <v>1014</v>
       </c>
+      <c r="K13" s="3" t="s">
+        <v>21</v>
+      </c>
       <c r="L13" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="M13" s="3" t="s">
-        <v>18</v>
+        <v>18</v>
+      </c>
+      <c r="M13" s="4">
+        <v>17</v>
       </c>
       <c r="N13" s="4">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="O13" s="4">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="P13" s="4">
-        <v>18</v>
-      </c>
-      <c r="Q13" s="4">
         <f t="shared" si="1"/>
         <v>16.666666666666668</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>1023</v>
       </c>
@@ -1414,44 +1371,43 @@
       <c r="C14" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="D14" s="3"/>
+      <c r="D14" s="4">
+        <v>17</v>
+      </c>
       <c r="E14" s="4">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="F14" s="4">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="G14" s="4">
-        <v>18</v>
-      </c>
-      <c r="H14" s="4">
         <f t="shared" si="0"/>
         <v>16.666666666666668</v>
       </c>
-      <c r="K14" s="2">
+      <c r="J14" s="2">
         <v>1023</v>
       </c>
+      <c r="K14" s="3" t="s">
+        <v>28</v>
+      </c>
       <c r="L14" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="M14" s="3" t="s">
         <v>24</v>
       </c>
+      <c r="M14" s="4">
+        <v>17</v>
+      </c>
       <c r="N14" s="4">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="O14" s="4">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="P14" s="4">
-        <v>18</v>
-      </c>
-      <c r="Q14" s="4">
         <f t="shared" si="1"/>
         <v>16.666666666666668</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>1017</v>
       </c>
@@ -1461,39 +1417,38 @@
       <c r="C15" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D15" s="3"/>
+      <c r="D15" s="4">
+        <v>15</v>
+      </c>
       <c r="E15" s="4">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="F15" s="4">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="G15" s="4">
-        <v>18</v>
-      </c>
-      <c r="H15" s="4">
         <f t="shared" si="0"/>
         <v>14.333333333333334</v>
       </c>
-      <c r="K15" s="2">
+      <c r="J15" s="2">
         <v>1017</v>
       </c>
+      <c r="K15" s="3" t="s">
+        <v>6</v>
+      </c>
       <c r="L15" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="M15" s="3" t="s">
         <v>7</v>
       </c>
+      <c r="M15" s="4">
+        <v>15</v>
+      </c>
       <c r="N15" s="4">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="O15" s="4">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="P15" s="4">
-        <v>18</v>
-      </c>
-      <c r="Q15" s="4">
         <f t="shared" si="1"/>
         <v>14.333333333333334</v>
       </c>

</xml_diff>